<commit_message>
update plots and interpre in EDA
</commit_message>
<xml_diff>
--- a/Data/Cardiovascular Disease.xlsx
+++ b/Data/Cardiovascular Disease.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Desktop\Master\P8105\Homework\Alzheimers_Disease_New_Hope\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF23AF5A-D278-4205-B938-5E0B43157B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13150D27-B0D4-4582-906F-E68637B16EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,18 +74,9 @@
     <t>Hawaii</t>
   </si>
   <si>
-    <t>ldaho</t>
-  </si>
-  <si>
-    <t>illinois</t>
-  </si>
-  <si>
     <t>Indiana</t>
   </si>
   <si>
-    <t>lowa</t>
-  </si>
-  <si>
     <t>Kansas</t>
   </si>
   <si>
@@ -189,6 +180,18 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Illinois</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iowa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -214,6 +217,7 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -533,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.45" x14ac:dyDescent="0.3"/>
@@ -763,7 +767,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B14" s="3">
         <v>0.06</v>
@@ -780,7 +784,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B15" s="3">
         <v>5.8999999999999997E-2</v>
@@ -797,7 +801,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3">
         <v>8.2000000000000003E-2</v>
@@ -814,7 +818,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B17" s="3">
         <v>6.5000000000000002E-2</v>
@@ -831,7 +835,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="3">
         <v>6.8000000000000005E-2</v>
@@ -848,7 +852,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3">
         <v>0.1</v>
@@ -865,7 +869,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3">
         <v>8.3000000000000004E-2</v>
@@ -882,7 +886,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3">
         <v>8.3000000000000004E-2</v>
@@ -899,7 +903,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3">
         <v>6.0999999999999999E-2</v>
@@ -916,7 +920,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3">
         <v>5.8000000000000003E-2</v>
@@ -933,7 +937,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3">
         <v>7.6999999999999999E-2</v>
@@ -950,7 +954,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" s="3">
         <v>5.6000000000000001E-2</v>
@@ -967,7 +971,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" s="3">
         <v>8.4000000000000005E-2</v>
@@ -984,7 +988,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27" s="3">
         <v>7.3999999999999996E-2</v>
@@ -1001,7 +1005,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" s="3">
         <v>6.8000000000000005E-2</v>
@@ -1018,7 +1022,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29" s="3">
         <v>5.8000000000000003E-2</v>
@@ -1035,7 +1039,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B30" s="3">
         <v>7.0000000000000007E-2</v>
@@ -1052,7 +1056,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B31" s="3">
         <v>6.0999999999999999E-2</v>
@@ -1069,7 +1073,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B32" s="3">
         <v>0.06</v>
@@ -1083,7 +1087,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B33" s="3">
         <v>6.2E-2</v>
@@ -1100,7 +1104,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B34" s="3">
         <v>6.2E-2</v>
@@ -1117,7 +1121,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B35" s="3">
         <v>8.1000000000000003E-2</v>
@@ -1134,7 +1138,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B36" s="3">
         <v>6.6000000000000003E-2</v>
@@ -1151,7 +1155,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B37" s="3">
         <v>7.9000000000000001E-2</v>
@@ -1168,7 +1172,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B38" s="3">
         <v>8.7999999999999995E-2</v>
@@ -1185,7 +1189,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B39" s="3">
         <v>7.0000000000000007E-2</v>
@@ -1202,7 +1206,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B40" s="3">
         <v>7.1999999999999995E-2</v>
@@ -1219,7 +1223,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B41" s="3">
         <v>7.0999999999999994E-2</v>
@@ -1236,7 +1240,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B42" s="3">
         <v>7.6999999999999999E-2</v>
@@ -1253,7 +1257,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B43" s="3">
         <v>7.0999999999999994E-2</v>
@@ -1270,7 +1274,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B44" s="3">
         <v>0.09</v>
@@ -1287,7 +1291,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B45" s="3">
         <v>6.7000000000000004E-2</v>
@@ -1304,7 +1308,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B46" s="3">
         <v>4.1000000000000002E-2</v>
@@ -1321,7 +1325,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B47" s="3">
         <v>6.0999999999999999E-2</v>
@@ -1338,7 +1342,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B48" s="3">
         <v>0.06</v>
@@ -1355,7 +1359,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B49" s="3">
         <v>5.8000000000000003E-2</v>
@@ -1372,7 +1376,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B50" s="3">
         <v>0.128</v>
@@ -1389,7 +1393,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B51" s="3">
         <v>5.8000000000000003E-2</v>
@@ -1406,7 +1410,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B52" s="3">
         <v>5.8000000000000003E-2</v>

</xml_diff>